<commit_message>
multiple row write in excel updated
</commit_message>
<xml_diff>
--- a/src/main/resources/exceltestdata/GBT.xlsx
+++ b/src/main/resources/exceltestdata/GBT.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\IdeaProjects\pega-automation-framework\src\main\resources\exceltestdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B234307B-68F0-4C46-8888-2B9A53D4C18B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A22F3A00-A776-4CD3-AFD6-08CD0201D616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="820" yWindow="-110" windowWidth="18490" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>RuleType</t>
   </si>
@@ -116,13 +116,26 @@
     <t>Expected</t>
   </si>
   <si>
+    <t>aff</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -493,23 +506,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="13" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="9" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.81640625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.0"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="24.81640625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.81640625"/>
+    <col min="5" max="13" bestFit="true" customWidth="true" width="7.81640625"/>
+    <col min="14" max="16" bestFit="true" customWidth="true" width="9.0"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="9.54296875"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="6.7265625"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="8.7265625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.35">
@@ -594,7 +607,7 @@
         <v>23</v>
       </c>
       <c r="S2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
@@ -605,6 +618,32 @@
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R5" t="s">
+        <v>30</v>
+      </c>
+      <c r="S5" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
code added if incorrect ruleName in file
</commit_message>
<xml_diff>
--- a/src/main/resources/exceltestdata/GBT.xlsx
+++ b/src/main/resources/exceltestdata/GBT.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\IdeaProjects\pega-automation-framework\src\main\resources\exceltestdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A22F3A00-A776-4CD3-AFD6-08CD0201D616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E823B0C1-8DFE-462B-B04A-21360CAEADD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="820" yWindow="-110" windowWidth="18490" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>RuleType</t>
   </si>
@@ -119,23 +119,13 @@
     <t>aff</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
-    <t>Fail</t>
+    <t>xyz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -508,21 +498,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2:S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.81640625"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.0"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="24.81640625"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.81640625"/>
-    <col min="5" max="13" bestFit="true" customWidth="true" width="7.81640625"/>
-    <col min="14" max="16" bestFit="true" customWidth="true" width="9.0"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="9.54296875"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="6.7265625"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="8.7265625"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="13" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.35">
@@ -592,7 +582,7 @@
         <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
@@ -602,12 +592,6 @@
       </c>
       <c r="Q2" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="R2" t="s">
-        <v>23</v>
-      </c>
-      <c r="S2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
@@ -638,12 +622,6 @@
       </c>
       <c r="Q5" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="R5" t="s">
-        <v>30</v>
-      </c>
-      <c r="S5" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sla related changes started
</commit_message>
<xml_diff>
--- a/src/main/resources/exceltestdata/GBT.xlsx
+++ b/src/main/resources/exceltestdata/GBT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\IdeaProjects\pega-automation-framework\src\main\resources\exceltestdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E823B0C1-8DFE-462B-B04A-21360CAEADD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FFEC958-37A6-4AFD-9037-BE82BA4D1289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="820" yWindow="-110" windowWidth="18490" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>RuleType</t>
   </si>
@@ -120,6 +120,15 @@
   </si>
   <si>
     <t>xyz</t>
+  </si>
+  <si>
+    <t>CAAssignService</t>
+  </si>
+  <si>
+    <t>PegaCS-Cases:08-06-01</t>
+  </si>
+  <si>
+    <t>PegaCA-Work-Service-GeneralRequest</t>
   </si>
 </sst>
 </file>
@@ -155,9 +164,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,8 +510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2:S5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -507,7 +519,7 @@
     <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="13" width="7.81640625" bestFit="1" customWidth="1"/>
     <col min="14" max="16" width="9" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9.54296875" bestFit="1" customWidth="1"/>
@@ -603,6 +615,15 @@
       <c r="A4" t="s">
         <v>25</v>
       </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" t="s">

</xml_diff>

<commit_message>
changed the whole search flow
</commit_message>
<xml_diff>
--- a/src/main/resources/exceltestdata/GBT.xlsx
+++ b/src/main/resources/exceltestdata/GBT.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\IdeaProjects\pega-automation-framework\src\main\resources\exceltestdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5521D0A-ACF0-4FCC-9A1F-8EA3AD948151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A73A73F-7420-4BD2-96BF-8555E930542F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="-110" windowWidth="18490" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="2580" windowWidth="13700" windowHeight="7810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GBT" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="33">
   <si>
     <t>RuleType</t>
   </si>
@@ -101,53 +101,43 @@
     <t>PegaFS:08-06-01</t>
   </si>
   <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>SLA</t>
+  </si>
+  <si>
+    <t>Expected</t>
+  </si>
+  <si>
+    <t>aff</t>
+  </si>
+  <si>
+    <t>TestSLA4</t>
+  </si>
+  <si>
+    <t>BFSCS:01-01-01</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>xyz</t>
+  </si>
+  <si>
     <t>BRO</t>
   </si>
   <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>Activity</t>
-  </si>
-  <si>
-    <t>SLA</t>
-  </si>
-  <si>
-    <t>Expected</t>
-  </si>
-  <si>
-    <t>aff</t>
-  </si>
-  <si>
-    <t>xyz</t>
-  </si>
-  <si>
-    <t>TestSLA4</t>
-  </si>
-  <si>
-    <t>BFSCS:01-01-01</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>RuleName not found</t>
+    <t>1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -528,23 +518,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.81640625"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.0"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="24.81640625"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="21.1796875"/>
-    <col min="5" max="13" bestFit="true" customWidth="true" width="7.81640625"/>
-    <col min="14" max="16" bestFit="true" customWidth="true" width="9.0"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="9.54296875"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="6.7265625"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="8.7265625"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="13" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.35">
@@ -597,7 +587,7 @@
         <v>15</v>
       </c>
       <c r="Q1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="R1" t="s">
         <v>16</v>
@@ -614,86 +604,77 @@
         <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
       </c>
       <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="R2" t="s">
-        <v>34</v>
-      </c>
-      <c r="S2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="R4" t="s">
-        <v>23</v>
-      </c>
-      <c r="S4" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
@@ -710,16 +691,136 @@
         <v>21</v>
       </c>
       <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
         <v>27</v>
       </c>
-      <c r="Q5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="R5" t="s">
-        <v>34</v>
-      </c>
-      <c r="S5" t="s">
-        <v>35</v>
+      <c r="D8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
results file created with datetime
</commit_message>
<xml_diff>
--- a/src/main/resources/exceltestdata/GBT.xlsx
+++ b/src/main/resources/exceltestdata/GBT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\IdeaProjects\pega-automation-framework\src\main\resources\exceltestdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10DB834C-3EA0-4483-B9FE-292A6456747D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9051F83F-3587-4DB2-92B9-94362198B0BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="2580" windowWidth="13700" windowHeight="7810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="820" yWindow="-110" windowWidth="18490" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GBT" sheetId="3" r:id="rId1"/>
@@ -532,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2:S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
updated code for Login in excel
</commit_message>
<xml_diff>
--- a/src/main/resources/exceltestdata/GBT.xlsx
+++ b/src/main/resources/exceltestdata/GBT.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\IdeaProjects\pega-automation-framework\src\main\resources\exceltestdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD3CCBF-2CAD-400A-AA01-8FF2C47E94AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9943A43A-DD8E-43CF-B7B8-CB357BE10726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="-110" windowWidth="18490" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="GBT" sheetId="3" r:id="rId1"/>
+    <sheet name="Login" sheetId="4" r:id="rId1"/>
+    <sheet name="GBT" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="49">
   <si>
     <t>RuleType</t>
   </si>
@@ -113,30 +114,18 @@
     <t>Expected</t>
   </si>
   <si>
-    <t>aff</t>
-  </si>
-  <si>
-    <t>TestSLA4</t>
-  </si>
-  <si>
     <t>BFSCS:01-01-01</t>
   </si>
   <si>
     <t>0</t>
   </si>
   <si>
-    <t>xyz</t>
-  </si>
-  <si>
     <t>BRO</t>
   </si>
   <si>
     <t>CAInitialSetUp</t>
   </si>
   <si>
-    <t>BFSCS_Branch_Changes:01-01-01</t>
-  </si>
-  <si>
     <t>MNTC-BFSCS-Work-Grp1-Interaction-InCorr</t>
   </si>
   <si>
@@ -149,16 +138,49 @@
     <t>AFF</t>
   </si>
   <si>
+    <t>RelatedPartyEnforcedEntry</t>
+  </si>
+  <si>
+    <t>WorkPendingDate</t>
+  </si>
+  <si>
+    <t>CheckListDueDate</t>
+  </si>
+  <si>
+    <t>DemographicUpdDate</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>https://bfs.maanticpegaservices.com/prweb</t>
+  </si>
+  <si>
+    <t>Navneet</t>
+  </si>
+  <si>
+    <t>rules</t>
+  </si>
+  <si>
+    <t>PegaAppCA:08-05-01</t>
+  </si>
+  <si>
+    <t>AppDetails</t>
+  </si>
+  <si>
+    <t>getURL</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
     <t>Pass</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>RuleName not found</t>
   </si>
 </sst>
 </file>
@@ -166,7 +188,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,16 +202,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -197,19 +241,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -226,9 +291,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -266,9 +331,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -301,26 +366,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -353,26 +401,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -545,27 +576,78 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:S9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79A5640B-F915-47DB-8E0E-2580AF62DB1F}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.81640625"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.0"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="24.81640625"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="21.1796875"/>
-    <col min="5" max="13" bestFit="true" customWidth="true" width="7.81640625"/>
-    <col min="14" max="16" bestFit="true" customWidth="true" width="9.0"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="9.54296875"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="6.7265625"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="8.7265625"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="37.88671875"/>
+    <col min="2" max="2" customWidth="true" width="37.88671875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.33203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{0E9F097B-9DFE-4F5C-83E2-FA6B4C75F79E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:S7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.77734375"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.0"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="24.77734375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="21.21875"/>
+    <col min="5" max="13" bestFit="true" customWidth="true" width="7.77734375"/>
+    <col min="14" max="16" bestFit="true" customWidth="true" width="9.0"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="9.5546875"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="6.77734375"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="8.77734375"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -624,7 +706,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -632,48 +714,42 @@
         <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="Q2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="R2" t="s">
-        <v>40</v>
-      </c>
-      <c r="S2" t="s">
-        <v>41</v>
-      </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="R3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="S3" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -681,52 +757,52 @@
         <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="Q4" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -740,33 +816,66 @@
         <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q6" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -774,124 +883,48 @@
         <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q8" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="R8" t="s">
-        <v>40</v>
-      </c>
-      <c r="S8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="O9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="P9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q9" s="3" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>